<commit_message>
verwerking winkelgebieden / kernwinkelgebieden 2021
- toevoegen files in standaardformaat
- technische wijzigingen in verwerkingslogica
</commit_message>
<xml_diff>
--- a/data_voor_swing/gebiedsdefinities/kernwinkelgebied.xlsx
+++ b/data_voor_swing/gebiedsdefinities/kernwinkelgebied.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,16 +415,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="23">
-        <v>10017</v>
+        <v>10018</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Zone Bonewijk-Grote Markt Aarschot</t>
+          <t>Zone Schaluin Aarschot</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Aarschot - Zone Bonewijk-Grote Markt Aarschot</t>
+          <t>Aarschot - Zone Schaluin Aarschot</t>
         </is>
       </c>
     </row>
@@ -433,16 +433,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="23">
-        <v>10018</v>
+        <v>10017</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Zone Schaluin Aarschot</t>
+          <t>Zone Bonewijk-Grote Markt Aarschot</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Aarschot - Zone Schaluin Aarschot</t>
+          <t>Aarschot - Zone Bonewijk-Grote Markt Aarschot</t>
         </is>
       </c>
     </row>
@@ -451,16 +451,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="23">
-        <v>10057</v>
+        <v>10071</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Abdijstraat-Den TIR Antwerpen</t>
+          <t>Linkeroever Antwerpen</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Antwerpen - Abdijstraat-Den TIR Antwerpen</t>
+          <t>Antwerpen - Linkeroever Antwerpen</t>
         </is>
       </c>
     </row>
@@ -469,16 +469,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="23">
-        <v>10058</v>
+        <v>10057</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Anselmo-Kasteelplein Antwerpen</t>
+          <t>Abdijstraat-Den TIR Antwerpen</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Antwerpen - Anselmo-Kasteelplein Antwerpen</t>
+          <t>Antwerpen - Abdijstraat-Den TIR Antwerpen</t>
         </is>
       </c>
     </row>
@@ -487,16 +487,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="23">
-        <v>10059</v>
+        <v>10058</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Antwerpen-Noord</t>
+          <t>Anselmo-Kasteelplein Antwerpen</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Antwerpen - Antwerpen-Noord</t>
+          <t>Antwerpen - Anselmo-Kasteelplein Antwerpen</t>
         </is>
       </c>
     </row>
@@ -505,16 +505,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="23">
-        <v>10060</v>
+        <v>10059</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Brederodewijk Antwerpen</t>
+          <t>Antwerpen-Noord</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Antwerpen - Brederodewijk Antwerpen</t>
+          <t>Antwerpen - Antwerpen-Noord</t>
         </is>
       </c>
     </row>
@@ -523,16 +523,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="23">
-        <v>10061</v>
+        <v>10060</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Centrum Antwerpen</t>
+          <t>Brederodewijk Antwerpen</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Antwerpen - Centrum Antwerpen</t>
+          <t>Antwerpen - Brederodewijk Antwerpen</t>
         </is>
       </c>
     </row>
@@ -541,16 +541,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="23">
-        <v>10062</v>
+        <v>10061</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Centrum Ekeren</t>
+          <t>Centrum Antwerpen</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Antwerpen - Centrum Ekeren</t>
+          <t>Antwerpen - Centrum Antwerpen</t>
         </is>
       </c>
     </row>
@@ -559,16 +559,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="23">
-        <v>10063</v>
+        <v>10062</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Centrum Hoboken</t>
+          <t>Centrum Ekeren</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Antwerpen - Centrum Hoboken</t>
+          <t>Antwerpen - Centrum Ekeren</t>
         </is>
       </c>
     </row>
@@ -577,16 +577,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="23">
-        <v>10064</v>
+        <v>10063</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Centrum Merksem</t>
+          <t>Centrum Hoboken</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Antwerpen - Centrum Merksem</t>
+          <t>Antwerpen - Centrum Hoboken</t>
         </is>
       </c>
     </row>
@@ -595,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="23">
-        <v>10065</v>
+        <v>10064</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Centrum Wilrijk</t>
+          <t>Centrum Merksem</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Antwerpen - Centrum Wilrijk</t>
+          <t>Antwerpen - Centrum Merksem</t>
         </is>
       </c>
     </row>
@@ -613,16 +613,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="23">
-        <v>10066</v>
+        <v>10065</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Deurne_Noord Antwerpen</t>
+          <t>Centrum Wilrijk</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Antwerpen - Deurne_Noord Antwerpen</t>
+          <t>Antwerpen - Centrum Wilrijk</t>
         </is>
       </c>
     </row>
@@ -631,16 +631,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="23">
-        <v>10067</v>
+        <v>10066</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Deurne_Zuid Antwerpen</t>
+          <t>Deurne-Noord Antwerpen</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Antwerpen - Deurne_Zuid Antwerpen</t>
+          <t>Antwerpen - Deurne-Noord Antwerpen</t>
         </is>
       </c>
     </row>
@@ -649,16 +649,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="23">
-        <v>10068</v>
+        <v>10067</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Driekoningenstraat-Statiestraat Antwerpen</t>
+          <t>Deurne-Zuid Antwerpen</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Antwerpen - Driekoningenstraat-Statiestraat Antwerpen</t>
+          <t>Antwerpen - Deurne-Zuid Antwerpen</t>
         </is>
       </c>
     </row>
@@ -667,16 +667,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="23">
-        <v>10069</v>
+        <v>10068</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Fruithoflaan Antwerpen</t>
+          <t>Driekoningenstraat-Statiestraat Antwerpen</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Antwerpen - Fruithoflaan Antwerpen</t>
+          <t>Antwerpen - Driekoningenstraat-Statiestraat Antwerpen</t>
         </is>
       </c>
     </row>
@@ -685,16 +685,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="23">
-        <v>10070</v>
+        <v>10069</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gitschotellei Antwerpen</t>
+          <t>Fruithoflaan Antwerpen</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Antwerpen - Gitschotellei Antwerpen</t>
+          <t>Antwerpen - Fruithoflaan Antwerpen</t>
         </is>
       </c>
     </row>
@@ -703,16 +703,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="23">
-        <v>10071</v>
+        <v>10070</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Linkeroever Antwerpen</t>
+          <t>Gitschotellei Antwerpen</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Antwerpen - Linkeroever Antwerpen</t>
+          <t>Antwerpen - Gitschotellei Antwerpen</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Turnhoutsebaan_Borgerhout Antwerpen</t>
+          <t>Turnhoutsebaan-Borgerhout Antwerpen</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Antwerpen - Turnhoutsebaan_Borgerhout Antwerpen</t>
+          <t>Antwerpen - Turnhoutsebaan-Borgerhout Antwerpen</t>
         </is>
       </c>
     </row>
@@ -779,12 +779,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Vlaamse_Waalsekaai Antwerpen</t>
+          <t>Vlaamse-Waalsekaai Antwerpen</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Antwerpen - Vlaamse_Waalsekaai Antwerpen</t>
+          <t>Antwerpen - Vlaamse-Waalsekaai Antwerpen</t>
         </is>
       </c>
     </row>
@@ -883,16 +883,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="23">
-        <v>10052</v>
+        <v>10162</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Centrum Deinze</t>
+          <t>Brugge</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Deinze - Centrum Deinze</t>
+          <t>Brugge - Brugge</t>
         </is>
       </c>
     </row>
@@ -901,16 +901,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="23">
-        <v>10016</v>
+        <v>10052</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Diest</t>
+          <t>Centrum Deinze</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Diest - Diest</t>
+          <t>Deinze - Centrum Deinze</t>
         </is>
       </c>
     </row>
@@ -919,16 +919,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="23">
-        <v>10092</v>
+        <v>10016</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Diksmuide</t>
+          <t>Diest</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Diksmuide - Diksmuide</t>
+          <t>Diest - Diest</t>
         </is>
       </c>
     </row>
@@ -937,16 +937,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="23">
-        <v>10130</v>
+        <v>10092</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Eeklo zone C</t>
+          <t>Diksmuide</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Eeklo - Eeklo zone C</t>
+          <t>Diksmuide - Diksmuide</t>
         </is>
       </c>
     </row>
@@ -955,16 +955,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="23">
-        <v>10131</v>
+        <v>10130</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Eeklo zone B</t>
+          <t>Eeklo zone C</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Eeklo - Eeklo zone B</t>
+          <t>Eeklo - Eeklo zone C</t>
         </is>
       </c>
     </row>
@@ -973,16 +973,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="23">
-        <v>10132</v>
+        <v>10131</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Eeklo zone A</t>
+          <t>Eeklo zone B</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Eeklo - Eeklo zone A</t>
+          <t>Eeklo - Eeklo zone B</t>
         </is>
       </c>
     </row>
@@ -991,16 +991,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="23">
-        <v>10079</v>
+        <v>10132</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Geel</t>
+          <t>Eeklo zone A</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Geel - Geel</t>
+          <t>Eeklo - Eeklo zone A</t>
         </is>
       </c>
     </row>
@@ -1009,16 +1009,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="23">
-        <v>10096</v>
+        <v>10079</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Centrum Genk</t>
+          <t>Geel</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Genk - Centrum Genk</t>
+          <t>Geel - Geel</t>
         </is>
       </c>
     </row>
@@ -1027,16 +1027,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="23">
-        <v>10097</v>
+        <v>10096</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Driehoeven Genk</t>
+          <t>Centrum Genk</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Genk - Driehoeven Genk</t>
+          <t>Genk - Centrum Genk</t>
         </is>
       </c>
     </row>
@@ -1045,16 +1045,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="23">
-        <v>10098</v>
+        <v>10097</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hoevenzavellaan Genk</t>
+          <t>Driehoeven Genk</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Genk - Hoevenzavellaan Genk</t>
+          <t>Genk - Driehoeven Genk</t>
         </is>
       </c>
     </row>
@@ -1063,16 +1063,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="23">
-        <v>10099</v>
+        <v>10098</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Koning Boudewijnlaan Genk</t>
+          <t>Hoevenzavellaan Genk</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Genk - Koning Boudewijnlaan Genk</t>
+          <t>Genk - Hoevenzavellaan Genk</t>
         </is>
       </c>
     </row>
@@ -1081,16 +1081,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="23">
-        <v>10100</v>
+        <v>10099</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Landwaartslaan Genk</t>
+          <t>Koning Boudewijnlaan Genk</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Genk - Landwaartslaan Genk</t>
+          <t>Genk - Koning Boudewijnlaan Genk</t>
         </is>
       </c>
     </row>
@@ -1099,16 +1099,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="23">
-        <v>10101</v>
+        <v>10100</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Stalenstraat Genk</t>
+          <t>Landwaartslaan Genk</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Genk - Stalenstraat Genk</t>
+          <t>Genk - Landwaartslaan Genk</t>
         </is>
       </c>
     </row>
@@ -1117,16 +1117,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="23">
-        <v>10102</v>
+        <v>10101</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Vennestraat Genk</t>
+          <t>Stalenstraat Genk</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Genk - Vennestraat Genk</t>
+          <t>Genk - Stalenstraat Genk</t>
         </is>
       </c>
     </row>
@@ -1135,16 +1135,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="23">
-        <v>10080</v>
+        <v>10102</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Geraardsbergen</t>
+          <t>Vennestraat Genk</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Geraardsbergen - Geraardsbergen</t>
+          <t>Genk - Vennestraat Genk</t>
         </is>
       </c>
     </row>
@@ -1153,16 +1153,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="23">
-        <v>10077</v>
+        <v>10080</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Glabbeek</t>
+          <t>Geraardsbergen</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Glabbeek - Glabbeek</t>
+          <t>Geraardsbergen - Geraardsbergen</t>
         </is>
       </c>
     </row>
@@ -1171,16 +1171,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="23">
-        <v>10081</v>
+        <v>10077</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Grobbendonk</t>
+          <t>Glabbeek</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Grobbendonk - Grobbendonk</t>
+          <t>Glabbeek - Glabbeek</t>
         </is>
       </c>
     </row>
@@ -1189,16 +1189,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="23">
-        <v>10049</v>
+        <v>10081</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Centrum Hamme</t>
+          <t>Grobbendonk</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Hamme - Centrum Hamme</t>
+          <t>Grobbendonk - Grobbendonk</t>
         </is>
       </c>
     </row>
@@ -1207,16 +1207,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="23">
-        <v>10106</v>
+        <v>10049</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Herentals</t>
+          <t>Centrum Hamme</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Herentals - Herentals</t>
+          <t>Hamme - Centrum Hamme</t>
         </is>
       </c>
     </row>
@@ -1225,16 +1225,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="23">
-        <v>10082</v>
+        <v>10106</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Herenthout</t>
+          <t>Herentals</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Herenthout - Herenthout</t>
+          <t>Herentals - Herentals</t>
         </is>
       </c>
     </row>
@@ -1243,16 +1243,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="23">
-        <v>10089</v>
+        <v>10082</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Herne</t>
+          <t>Herenthout</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Herne - Herne</t>
+          <t>Herenthout - Herenthout</t>
         </is>
       </c>
     </row>
@@ -1261,16 +1261,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="23">
-        <v>10103</v>
+        <v>10089</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>'Cité' Heusden-Zolder</t>
+          <t>Herne</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Heusden-Zolder - 'Cité' Heusden-Zolder</t>
+          <t>Herne - Herne</t>
         </is>
       </c>
     </row>
@@ -1279,16 +1279,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="23">
-        <v>10148</v>
+        <v>10103</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Hoeilaart</t>
+          <t>'Cité' Heusden-Zolder</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Hoeilaart - Hoeilaart</t>
+          <t>Heusden-Zolder - 'Cité' Heusden-Zolder</t>
         </is>
       </c>
     </row>
@@ -1297,16 +1297,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="23">
-        <v>10094</v>
+        <v>10148</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ieper</t>
+          <t>Hoeilaart</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Ieper - Ieper</t>
+          <t>Hoeilaart - Hoeilaart</t>
         </is>
       </c>
     </row>
@@ -1315,16 +1315,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="23">
-        <v>10158</v>
+        <v>10094</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Izegem</t>
+          <t>Ieper</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Izegem - Izegem</t>
+          <t>Ieper - Ieper</t>
         </is>
       </c>
     </row>
@@ -1333,16 +1333,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="23">
-        <v>10135</v>
+        <v>10158</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Heist-Centrum</t>
+          <t>Izegem</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Knokke-Heist - Heist-Centrum</t>
+          <t>Izegem - Izegem</t>
         </is>
       </c>
     </row>
@@ -1351,16 +1351,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="23">
-        <v>10147</v>
+        <v>10155</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Gouden driehoek Knokke</t>
+          <t>Knokke-HeistZone A</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Knokke-Heist - Gouden driehoek Knokke</t>
+          <t>Knokke-Heist - Knokke-HeistZone A</t>
         </is>
       </c>
     </row>
@@ -1369,16 +1369,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="23">
-        <v>10001</v>
+        <v>10044</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Kortrijk</t>
+          <t>Centrum Kooigem</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Kortrijk - Kortrijk</t>
+          <t>Kortrijk - Centrum Kooigem</t>
         </is>
       </c>
     </row>
@@ -1387,16 +1387,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="23">
-        <v>10041</v>
+        <v>10042</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Overleie Kortrijk</t>
+          <t>Centrum Rollegem</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Kortrijk - Overleie Kortrijk</t>
+          <t>Kortrijk - Centrum Rollegem</t>
         </is>
       </c>
     </row>
@@ -1405,16 +1405,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="23">
-        <v>10042</v>
+        <v>10047</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Centrum Rollegem</t>
+          <t>Centrum Bellegem</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Rollegem</t>
+          <t>Kortrijk - Centrum Bellegem</t>
         </is>
       </c>
     </row>
@@ -1423,16 +1423,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="23">
-        <v>10043</v>
+        <v>10048</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Centrum Marke</t>
+          <t>Centrum Aalbeke</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Marke</t>
+          <t>Kortrijk - Centrum Aalbeke</t>
         </is>
       </c>
     </row>
@@ -1441,16 +1441,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="23">
-        <v>10044</v>
+        <v>10043</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Centrum Kooigem</t>
+          <t>Centrum Marke</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Kooigem</t>
+          <t>Kortrijk - Centrum Marke</t>
         </is>
       </c>
     </row>
@@ -1459,16 +1459,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="23">
-        <v>10045</v>
+        <v>10046</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Centrum Heule</t>
+          <t>Centrum Bissegem</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Heule</t>
+          <t>Kortrijk - Centrum Bissegem</t>
         </is>
       </c>
     </row>
@@ -1477,16 +1477,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="23">
-        <v>10046</v>
+        <v>10001</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Centrum Bissegem</t>
+          <t>Kortrijk</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Bissegem</t>
+          <t>Kortrijk - Kortrijk</t>
         </is>
       </c>
     </row>
@@ -1495,16 +1495,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="23">
-        <v>10047</v>
+        <v>10045</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Centrum Bellegem</t>
+          <t>Centrum Heule</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Bellegem</t>
+          <t>Kortrijk - Centrum Heule</t>
         </is>
       </c>
     </row>
@@ -1513,16 +1513,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="23">
-        <v>10048</v>
+        <v>10041</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Centrum Aalbeke</t>
+          <t>Overleie Kortrijk</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Kortrijk - Centrum Aalbeke</t>
+          <t>Kortrijk - Overleie Kortrijk</t>
         </is>
       </c>
     </row>
@@ -1625,12 +1625,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Liederkerke</t>
+          <t>Liedekerke</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Liedekerke - Liederkerke</t>
+          <t>Liedekerke - Liedekerke</t>
         </is>
       </c>
     </row>
@@ -1783,16 +1783,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="23">
-        <v>10104</v>
+        <v>10163</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Poperingen</t>
+          <t>Belle Epoque</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Poperinge - Poperingen</t>
+          <t>Oostende - Belle Epoque</t>
         </is>
       </c>
     </row>
@@ -1801,16 +1801,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="23">
-        <v>10108</v>
+        <v>10164</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Puurs</t>
+          <t>Centrum Oostende</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Puurs-Sint-Amands - Puurs</t>
+          <t>Oostende - Centrum Oostende</t>
         </is>
       </c>
     </row>
@@ -1819,16 +1819,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="23">
-        <v>10002</v>
+        <v>10104</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Roeselare</t>
+          <t>Poperinge</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Roeselare - Roeselare</t>
+          <t>Poperinge - Poperinge</t>
         </is>
       </c>
     </row>
@@ -1837,16 +1837,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="23">
-        <v>10050</v>
+        <v>10108</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Centrum Ronse</t>
+          <t>Puurs</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Ronse - Centrum Ronse</t>
+          <t>Puurs-Sint-Amands - Puurs</t>
         </is>
       </c>
     </row>
@@ -1855,16 +1855,16 @@
         <v>81</v>
       </c>
       <c r="B82" s="23">
-        <v>10086</v>
+        <v>10160</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Terhagen Rumst</t>
+          <t>Roeselare</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Rumst - Terhagen Rumst</t>
+          <t>Roeselare - Roeselare</t>
         </is>
       </c>
     </row>
@@ -1873,16 +1873,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="23">
-        <v>10087</v>
+        <v>10161</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Rumst</t>
+          <t>Roeselare uitbreiding</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Rumst - Rumst</t>
+          <t>Roeselare - Roeselare uitbreiding</t>
         </is>
       </c>
     </row>
@@ -1891,16 +1891,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="23">
-        <v>10088</v>
+        <v>10050</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Reet Rumst</t>
+          <t>Centrum Ronse</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Rumst - Reet Rumst</t>
+          <t>Ronse - Centrum Ronse</t>
         </is>
       </c>
     </row>
@@ -1909,16 +1909,16 @@
         <v>84</v>
       </c>
       <c r="B85" s="23">
-        <v>10127</v>
+        <v>10086</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Schoten Categorie A</t>
+          <t>Terhagen Rumst</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Schoten - Schoten Categorie A</t>
+          <t>Rumst - Terhagen Rumst</t>
         </is>
       </c>
     </row>
@@ -1927,16 +1927,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="23">
-        <v>10128</v>
+        <v>10087</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Schoten Categorie B</t>
+          <t>Rumst</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Schoten - Schoten Categorie B</t>
+          <t>Rumst - Rumst</t>
         </is>
       </c>
     </row>
@@ -1945,16 +1945,16 @@
         <v>86</v>
       </c>
       <c r="B87" s="23">
-        <v>10129</v>
+        <v>10088</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Schoten Categorie C</t>
+          <t>Reet Rumst</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Schoten - Schoten Categorie C</t>
+          <t>Rumst - Reet Rumst</t>
         </is>
       </c>
     </row>
@@ -1963,16 +1963,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="23">
-        <v>10116</v>
+        <v>10127</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Middenhut en Parvis Sint-Genesius-Rode</t>
+          <t>Schoten Categorie A</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Sint-Genesius-Rode - Middenhut en Parvis Sint-Genesius-Rode</t>
+          <t>Schoten - Schoten Categorie A</t>
         </is>
       </c>
     </row>
@@ -1981,16 +1981,16 @@
         <v>88</v>
       </c>
       <c r="B89" s="23">
-        <v>10117</v>
+        <v>10128</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Waterloosesteenweg Sint-Genesius-Rode</t>
+          <t>Schoten Categorie B</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Sint-Genesius-Rode - Waterloosesteenweg Sint-Genesius-Rode</t>
+          <t>Schoten - Schoten Categorie B</t>
         </is>
       </c>
     </row>
@@ -1999,16 +1999,16 @@
         <v>89</v>
       </c>
       <c r="B90" s="23">
-        <v>10118</v>
+        <v>10129</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Steenweg naar Halle Sint-Genesius-Rode</t>
+          <t>Schoten Categorie C</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Sint-Genesius-Rode - Steenweg naar Halle Sint-Genesius-Rode</t>
+          <t>Schoten - Schoten Categorie C</t>
         </is>
       </c>
     </row>
@@ -2017,16 +2017,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="23">
-        <v>10119</v>
+        <v>10116</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Centrum Sint-Genesius-Rode</t>
+          <t>Middenhut en Parvis Sint-Genesius-Rode</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Sint-Genesius-Rode - Centrum Sint-Genesius-Rode</t>
+          <t>Sint-Genesius-Rode - Middenhut en Parvis Sint-Genesius-Rode</t>
         </is>
       </c>
     </row>
@@ -2035,16 +2035,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="23">
-        <v>10091</v>
+        <v>10117</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Sint-Niklaas</t>
+          <t>Waterloosesteenweg Sint-Genesius-Rode</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Sint-Niklaas - Sint-Niklaas</t>
+          <t>Sint-Genesius-Rode - Waterloosesteenweg Sint-Genesius-Rode</t>
         </is>
       </c>
     </row>
@@ -2053,16 +2053,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="23">
-        <v>10126</v>
+        <v>10118</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Focusgebied</t>
+          <t>Steenweg naar Halle Sint-Genesius-Rode</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Sint-Niklaas - Focusgebied</t>
+          <t>Sint-Genesius-Rode - Steenweg naar Halle Sint-Genesius-Rode</t>
         </is>
       </c>
     </row>
@@ -2071,16 +2071,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="23">
-        <v>10111</v>
+        <v>10119</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Sint-Truiden</t>
+          <t>Centrum Sint-Genesius-Rode</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Sint-Truiden - Sint-Truiden</t>
+          <t>Sint-Genesius-Rode - Centrum Sint-Genesius-Rode</t>
         </is>
       </c>
     </row>
@@ -2089,16 +2089,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="23">
-        <v>10005</v>
+        <v>10091</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Tervuren</t>
+          <t>Sint-Niklaas</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Tervuren - Tervuren</t>
+          <t>Sint-Niklaas - Sint-Niklaas</t>
         </is>
       </c>
     </row>
@@ -2107,16 +2107,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="23">
-        <v>10003</v>
+        <v>10126</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Tielt</t>
+          <t>Focusgebied</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Tielt - Tielt</t>
+          <t>Sint-Niklaas - Focusgebied</t>
         </is>
       </c>
     </row>
@@ -2125,16 +2125,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="23">
-        <v>10095</v>
+        <v>10111</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Torhout</t>
+          <t>Sint-Truiden</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Torhout - Torhout</t>
+          <t>Sint-Truiden - Sint-Truiden</t>
         </is>
       </c>
     </row>
@@ -2143,16 +2143,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="23">
-        <v>10078</v>
+        <v>10005</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Turnhout</t>
+          <t>Tervuren</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Turnhout - Turnhout</t>
+          <t>Tervuren - Tervuren</t>
         </is>
       </c>
     </row>
@@ -2161,16 +2161,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="23">
-        <v>10015</v>
+        <v>10003</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Vilvoorde</t>
+          <t>Tielt</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Vilvoorde - Vilvoorde</t>
+          <t>Tielt - Tielt</t>
         </is>
       </c>
     </row>
@@ -2179,16 +2179,16 @@
         <v>99</v>
       </c>
       <c r="B100" s="23">
-        <v>10121</v>
+        <v>10095</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Geluwe</t>
+          <t>Torhout</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Wervik - Geluwe</t>
+          <t>Torhout - Torhout</t>
         </is>
       </c>
     </row>
@@ -2197,16 +2197,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="23">
-        <v>10122</v>
+        <v>10078</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Wervik</t>
+          <t>Turnhout</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Wervik - Wervik</t>
+          <t>Turnhout - Turnhout</t>
         </is>
       </c>
     </row>
@@ -2215,16 +2215,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="23">
-        <v>10105</v>
+        <v>10015</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Willebroek</t>
+          <t>Vilvoorde</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Willebroek - Willebroek</t>
+          <t>Vilvoorde - Vilvoorde</t>
         </is>
       </c>
     </row>
@@ -2233,16 +2233,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="23">
-        <v>10053</v>
+        <v>10159</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Dorpskern Laar - woonkernzone Zemst</t>
+          <t>Vosselaar</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Zemst - Dorpskern Laar - woonkernzone Zemst</t>
+          <t>Vosselaar - Vosselaar</t>
         </is>
       </c>
     </row>
@@ -2251,16 +2251,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="23">
-        <v>10054</v>
+        <v>10121</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Kleinhandelszone Weerde Zemst</t>
+          <t>Geluwe</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Zemst - Kleinhandelszone Weerde Zemst</t>
+          <t>Wervik - Geluwe</t>
         </is>
       </c>
     </row>
@@ -2269,16 +2269,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="23">
-        <v>10019</v>
+        <v>10122</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>8550 Zwevegem</t>
+          <t>Wervik</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Zwevegem - 8550 Zwevegem</t>
+          <t>Wervik - Wervik</t>
         </is>
       </c>
     </row>
@@ -2287,16 +2287,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="23">
-        <v>10020</v>
+        <v>10105</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>8551 Heestert Zwevegem</t>
+          <t>Willebroek</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Zwevegem - 8551 Heestert Zwevegem</t>
+          <t>Willebroek - Willebroek</t>
         </is>
       </c>
     </row>
@@ -2305,16 +2305,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="23">
-        <v>10021</v>
+        <v>10053</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>8552 Moen Zwevegem</t>
+          <t>Dorpskern Laar - woonkernzone Zemst</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Zwevegem - 8552 Moen Zwevegem</t>
+          <t>Zemst - Dorpskern Laar - woonkernzone Zemst</t>
         </is>
       </c>
     </row>
@@ -2323,16 +2323,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="23">
-        <v>10023</v>
+        <v>10054</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>8553 Otegem Zwevegem</t>
+          <t>Kleinhandelszone Weerde Zemst</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Zwevegem - 8553 Otegem Zwevegem</t>
+          <t>Zemst - Kleinhandelszone Weerde Zemst</t>
         </is>
       </c>
     </row>
@@ -2341,16 +2341,16 @@
         <v>108</v>
       </c>
       <c r="B109" s="23">
-        <v>10024</v>
+        <v>10020</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>8554 Sint-Denijs Zwevegem</t>
+          <t>8551 Heestert Zwevegem</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Zwevegem - 8554 Sint-Denijs Zwevegem</t>
+          <t>Zwevegem - 8551 Heestert Zwevegem</t>
         </is>
       </c>
     </row>
@@ -2359,16 +2359,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="23">
-        <v>10107</v>
+        <v>10021</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Zwijndrecht</t>
+          <t>8552 Moen Zwevegem</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Zwijndrecht - Zwijndrecht</t>
+          <t>Zwevegem - 8552 Moen Zwevegem</t>
         </is>
       </c>
     </row>
@@ -2377,14 +2377,86 @@
         <v>110</v>
       </c>
       <c r="B111" s="23">
+        <v>10023</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>8553 Otegem Zwevegem</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Zwevegem - 8553 Otegem Zwevegem</t>
+        </is>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="0" outlineLevel="0">
+      <c r="A112" s="23">
+        <v>111</v>
+      </c>
+      <c r="B112" s="23">
+        <v>10024</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>8554 Sint-Denijs Zwevegem</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Zwevegem - 8554 Sint-Denijs Zwevegem</t>
+        </is>
+      </c>
+    </row>
+    <row r="113" spans="1:4" s="0" outlineLevel="0">
+      <c r="A113" s="23">
+        <v>112</v>
+      </c>
+      <c r="B113" s="23">
+        <v>10019</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>8550 Zwevegem</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Zwevegem - 8550 Zwevegem</t>
+        </is>
+      </c>
+    </row>
+    <row r="114" spans="1:4" s="0" outlineLevel="0">
+      <c r="A114" s="23">
+        <v>113</v>
+      </c>
+      <c r="B114" s="23">
+        <v>10107</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Zwijndrecht</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Zwijndrecht - Zwijndrecht</t>
+        </is>
+      </c>
+    </row>
+    <row r="115" spans="1:4" s="0" outlineLevel="0">
+      <c r="A115" s="23">
+        <v>114</v>
+      </c>
+      <c r="B115" s="23">
         <v>10110</v>
       </c>
-      <c r="C111" t="inlineStr">
+      <c r="C115" t="inlineStr">
         <is>
           <t>Stimuleringsgebied Burcht Zwijndrecht</t>
         </is>
       </c>
-      <c r="D111" t="inlineStr">
+      <c r="D115" t="inlineStr">
         <is>
           <t>Zwijndrecht - Stimuleringsgebied Burcht Zwijndrecht</t>
         </is>

</xml_diff>